<commit_message>
ending it for today
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ee7b7f860d2e05b/Documents/Financial Modelling Package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{F71E3C00-6F4D-4522-AA49-31643000A435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6535508-A34A-4AF7-880E-C3C5606B94F9}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{F71E3C00-6F4D-4522-AA49-31643000A435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0128D482-A8AB-4F01-99CF-46AF9EA50C91}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="30960" windowHeight="12204" xr2:uid="{237C08A7-68D0-4C3B-99C6-956D5D77C08B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="16680" xr2:uid="{237C08A7-68D0-4C3B-99C6-956D5D77C08B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21970,6 +21970,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22291,11 +22295,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A392417-B9AC-4A90-ACBB-9D0DE94AB6E7}">
   <dimension ref="A1:AO747"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AN4" sqref="AN4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>